<commit_message>
reponsive thêm trang index + update file task
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="20496" windowHeight="7895"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mitsg4nKYzU0T1mG+CZd0js0eHfeQ=="/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -51,16 +49,10 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Header</t>
+    <t>Home + Contact + Vercel + Github</t>
   </si>
   <si>
-    <t>12/13</t>
-  </si>
-  <si>
-    <t>Dev1</t>
-  </si>
-  <si>
-    <t>Dev2</t>
+    <t>Nguyễn Hoàng Quốc Hải</t>
   </si>
   <si>
     <t xml:space="preserve">     Logo</t>
@@ -84,55 +76,225 @@
     <t xml:space="preserve">      Login popup</t>
   </si>
   <si>
-    <t>Carousel</t>
+    <t>About + Blog Spots + Youtube</t>
+  </si>
+  <si>
+    <t>Trần Thành Lộc</t>
+  </si>
+  <si>
+    <t>404 Page</t>
+  </si>
+  <si>
+    <t>Nguyễn Đỗ Anh Tuấn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="mm/dd"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="26">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF363636"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -164,9 +326,201 @@
         <bgColor rgb="FFAEABAB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
-    <border/>
+  <borders count="16">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -180,6 +534,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -194,34 +549,37 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -230,12 +588,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -244,108 +601,390 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="6" fontId="3" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="6" fontId="3" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="3" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="3" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="5" fillId="5" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -358,18 +997,19 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -559,32 +1199,37 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:J986"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.5"/>
-    <col customWidth="1" min="2" max="4" width="7.63"/>
-    <col customWidth="1" min="5" max="5" width="10.25"/>
-    <col customWidth="1" min="6" max="6" width="7.63"/>
-    <col customWidth="1" min="7" max="7" width="9.25"/>
-    <col customWidth="1" min="8" max="8" width="7.63"/>
-    <col customWidth="1" min="9" max="9" width="8.75"/>
-    <col customWidth="1" min="10" max="10" width="33.0"/>
-    <col customWidth="1" min="11" max="26" width="7.63"/>
+    <col min="1" max="1" width="21.1" customWidth="1"/>
+    <col min="2" max="2" width="11.7" customWidth="1"/>
+    <col min="3" max="3" width="10.1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="8.8" customWidth="1"/>
+    <col min="7" max="7" width="13.6" customWidth="1"/>
+    <col min="8" max="8" width="5" customWidth="1"/>
+    <col min="9" max="9" width="17.2" customWidth="1"/>
+    <col min="10" max="10" width="33" customWidth="1"/>
+    <col min="11" max="26" width="7.63333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25.5" customHeight="1">
+    <row r="1" ht="24" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,278 +1254,286 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="21.75" customHeight="1" collapsed="1">
-      <c r="A2" s="7" t="s">
+    <row r="2" ht="13.8" collapsed="1" spans="1:10">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8">
-        <v>44175.0</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="6">
+        <v>45047</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45051</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="6">
+        <v>45053</v>
+      </c>
+      <c r="G2" s="6">
+        <v>45053</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" spans="1:10">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="8">
-        <v>44179.0</v>
-      </c>
-      <c r="H2" s="13">
-        <v>0.95</v>
-      </c>
-      <c r="I2" s="11" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="14"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
+        <v>44179</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="21"/>
     </row>
-    <row r="3" ht="14.25" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="17" t="s">
+    <row r="4" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" spans="1:10">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="8">
-        <v>44179.0</v>
-      </c>
-      <c r="H3" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" ht="14.25" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="12">
-        <v>43608.0</v>
-      </c>
-      <c r="C4" s="12">
-        <v>43647.0</v>
-      </c>
-      <c r="D4" s="20">
+      <c r="B4" s="6">
+        <v>43608</v>
+      </c>
+      <c r="C4" s="6">
+        <v>43647</v>
+      </c>
+      <c r="D4" s="14">
         <f>SUM(D5:D7)/3</f>
         <v>0.9</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="8">
-        <v>44179.0</v>
-      </c>
-      <c r="H4" s="21">
+      <c r="E4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <v>44179</v>
+      </c>
+      <c r="H4" s="15">
         <f>SUM(H5:H7)/3</f>
         <v>0.9</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="21"/>
+    </row>
+    <row r="5" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" spans="1:10">
+      <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="B5" s="16">
+        <v>43608</v>
+      </c>
+      <c r="C5" s="16">
+        <v>43616</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="6">
+        <v>44179</v>
+      </c>
+      <c r="H5" s="15">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="21"/>
     </row>
-    <row r="5" ht="14.25" hidden="1" customHeight="1" outlineLevel="2">
-      <c r="A5" s="15" t="s">
+    <row r="6" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" spans="1:10">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="16">
+        <v>43636</v>
+      </c>
+      <c r="C6" s="16">
+        <v>43644</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="6">
+        <v>44179</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="21"/>
+    </row>
+    <row r="7" ht="9" hidden="1" customHeight="1" outlineLevel="2" spans="1:10">
+      <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="22">
-        <v>43608.0</v>
-      </c>
-      <c r="C5" s="22">
-        <v>43616.0</v>
-      </c>
-      <c r="D5" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="8">
-        <v>44179.0</v>
-      </c>
-      <c r="H5" s="21">
-        <v>1.0</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="14"/>
+      <c r="B7" s="16">
+        <v>43641</v>
+      </c>
+      <c r="C7" s="16">
+        <v>43647</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="6">
+        <v>44179</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="22"/>
     </row>
-    <row r="6" ht="14.25" hidden="1" customHeight="1" outlineLevel="2">
-      <c r="A6" s="15" t="s">
+    <row r="8" ht="13.8" spans="1:10">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="22">
-        <v>43636.0</v>
-      </c>
-      <c r="C6" s="22">
-        <v>43644.0</v>
-      </c>
-      <c r="D6" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="8">
-        <v>44179.0</v>
-      </c>
-      <c r="H6" s="21">
-        <v>0.9</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="14"/>
+      <c r="B8" s="6">
+        <v>45047</v>
+      </c>
+      <c r="C8" s="7">
+        <v>45051</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="6">
+        <v>45053</v>
+      </c>
+      <c r="G8" s="6">
+        <v>45053</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="21"/>
     </row>
-    <row r="7" ht="9.0" hidden="1" customHeight="1" outlineLevel="2">
-      <c r="A7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="22">
-        <v>43641.0</v>
-      </c>
-      <c r="C7" s="22">
-        <v>43647.0</v>
-      </c>
-      <c r="D7" s="20">
-        <v>0.8</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="8">
-        <v>44179.0</v>
-      </c>
-      <c r="H7" s="21">
-        <v>0.8</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="23"/>
+    <row r="9" ht="13.8" spans="1:10">
+      <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="21"/>
     </row>
-    <row r="8">
-      <c r="A8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="8">
-        <v>44175.0</v>
-      </c>
-      <c r="C8" s="8">
-        <v>44178.0</v>
-      </c>
-      <c r="D8" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="8">
-        <v>44179.0</v>
-      </c>
-      <c r="H8" s="13">
-        <v>1.0</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="14"/>
+    <row r="10" ht="14.25" customHeight="1" spans="1:10">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="21"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="14"/>
+    <row r="11" ht="14.25" customHeight="1" spans="1:10">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="21"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="14"/>
+    <row r="12" ht="14.25" customHeight="1" spans="1:10">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="21"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="14"/>
+    <row r="13" ht="14.25" customHeight="1" spans="1:10">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="21"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="14"/>
+    <row r="14" ht="14.25" customHeight="1" spans="1:10">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" ht="14.25" customHeight="1"/>
     <row r="16" ht="14.25" customHeight="1"/>
@@ -1855,19 +2508,18 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="D2 D4:D14">
+  <conditionalFormatting sqref="D2;D4:D14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2 H4:H14">
+  <conditionalFormatting sqref="H2;H4:H14">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>